<commit_message>
Cause server not to give an error when data exists outside the matrix.
</commit_message>
<xml_diff>
--- a/test-files/graph-tests/dCIN5GendronModel1.xlsx
+++ b/test-files/graph-tests/dCIN5GendronModel1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14520" tabRatio="929" activeTab="4"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">dcin5!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -4768,8 +4768,8 @@
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>